<commit_message>
RESTORE BUT NEED MORE TESTS AND DEBUG
</commit_message>
<xml_diff>
--- a/REVs/REV-07-04-2025.xlsx
+++ b/REVs/REV-07-04-2025.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R212"/>
+  <dimension ref="A1:R215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10419,20 +10419,161 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I212" t="inlineStr"/>
       <c r="J212" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
         </is>
       </c>
-      <c r="K212" t="inlineStr"/>
-      <c r="L212" t="inlineStr"/>
-      <c r="M212" t="inlineStr"/>
-      <c r="N212" t="inlineStr"/>
-      <c r="O212" t="inlineStr"/>
-      <c r="P212" t="inlineStr"/>
-      <c r="Q212" t="inlineStr"/>
-      <c r="R212" t="inlineStr"/>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>0TN03011</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>CALLIDERM CREME MAINS &amp; ONGLES</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>TRATAMIENTO CUERPO MANOS</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>No Tiene ES - TRADUCIDO</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="H213" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J213" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>0TF23303</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>THE SKIN HOUSE WRINKLE SYSTEM CREAM 30 G</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>TRAT.FEMENINO</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>No Tiene ES - TRADUCIDO</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J214" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>0TF27023</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>THE SKIN HOUSE WRINKLE SYSTEM CREAM 50GR</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>TRAT.FEMENINO</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="I215" t="inlineStr"/>
+      <c r="J215" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+      <c r="K215" t="inlineStr"/>
+      <c r="L215" t="inlineStr"/>
+      <c r="M215" t="inlineStr"/>
+      <c r="N215" t="inlineStr"/>
+      <c r="O215" t="inlineStr"/>
+      <c r="P215" t="inlineStr"/>
+      <c r="Q215" t="inlineStr"/>
+      <c r="R215" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>